<commit_message>
Trained all basic models
</commit_message>
<xml_diff>
--- a/models_metrics.xlsx
+++ b/models_metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/891c7dffdadbb264/Área de Trabalho/attention_for_pose_estimation_github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_2B59D2BFD31055AB33AC39505A3088B35299F3C0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C485E26F-8D8E-4B7D-A845-4F019FB45FFD}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_2B59D2BFD310D5B08BDB9D714B3088B35299F4B0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8632C215-2F4A-4CCE-B22A-DD377F94410E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Model</t>
   </si>
@@ -40,22 +40,106 @@
     <t>Update</t>
   </si>
   <si>
-    <t>Baseline ResNet50 FC</t>
-  </si>
-  <si>
-    <t>27.94</t>
-  </si>
-  <si>
-    <t>41.10</t>
-  </si>
-  <si>
-    <t>90.94</t>
-  </si>
-  <si>
-    <t>78.75</t>
-  </si>
-  <si>
-    <t>2025-01-05 20:50:29</t>
+    <t>ResNet50 SAM Conv-Deconv</t>
+  </si>
+  <si>
+    <t>ResNet50 + CSA + Conv-Dec</t>
+  </si>
+  <si>
+    <t>21.68</t>
+  </si>
+  <si>
+    <t>61.62</t>
+  </si>
+  <si>
+    <t>67.72</t>
+  </si>
+  <si>
+    <t>67.66</t>
+  </si>
+  <si>
+    <t>2025-01-15 10:59:59</t>
+  </si>
+  <si>
+    <t>26.85</t>
+  </si>
+  <si>
+    <t>57.32</t>
+  </si>
+  <si>
+    <t>69.69</t>
+  </si>
+  <si>
+    <t>68.58</t>
+  </si>
+  <si>
+    <t>15-01-2025 40:16</t>
+  </si>
+  <si>
+    <t>29.88</t>
+  </si>
+  <si>
+    <t>45.57</t>
+  </si>
+  <si>
+    <t>93.68</t>
+  </si>
+  <si>
+    <t>83.22</t>
+  </si>
+  <si>
+    <t>2025-01-16 13:45:32</t>
+  </si>
+  <si>
+    <t>ResNet50 FC Base</t>
+  </si>
+  <si>
+    <t>28.85</t>
+  </si>
+  <si>
+    <t>37.83</t>
+  </si>
+  <si>
+    <t>97.88</t>
+  </si>
+  <si>
+    <t>70.49</t>
+  </si>
+  <si>
+    <t>ResNet50 FC SAM 1</t>
+  </si>
+  <si>
+    <t>ResNet50 FC CSA 1</t>
+  </si>
+  <si>
+    <t>30.15</t>
+  </si>
+  <si>
+    <t>42.38</t>
+  </si>
+  <si>
+    <t>61.35</t>
+  </si>
+  <si>
+    <t>68.78</t>
+  </si>
+  <si>
+    <t>ResNet50 Conv/Deconv</t>
+  </si>
+  <si>
+    <t>Retrain, with initialized positional encoding.</t>
+  </si>
+  <si>
+    <t>29.55</t>
+  </si>
+  <si>
+    <t>39.35</t>
+  </si>
+  <si>
+    <t>62.55</t>
+  </si>
+  <si>
+    <t>68.39</t>
   </si>
 </sst>
 </file>
@@ -74,6 +158,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,11 +196,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,23 +504,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,24 +538,127 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45675</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45676</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45677</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>